<commit_message>
More mismatched examples for configErrors file
</commit_message>
<xml_diff>
--- a/Example/ConfigErrors.xlsx
+++ b/Example/ConfigErrors.xlsx
@@ -13,12 +13,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
   <si>
     <t>Type of Entry</t>
   </si>
   <si>
     <t>Instructor</t>
+  </si>
+  <si>
+    <t>Course Name</t>
   </si>
   <si>
     <t>Excel Entry</t>
@@ -27,10 +30,22 @@
     <t>lllllll</t>
   </si>
   <si>
+    <t>John</t>
+  </si>
+  <si>
+    <t>MATH 101</t>
+  </si>
+  <si>
     <t>File Path</t>
   </si>
   <si>
     <t>Distribution Files\F1997\MEC E 260 - 502 (77588) Ayranci\MecE260_UNDERGRAD Grade Dist Form.xlsx</t>
+  </si>
+  <si>
+    <t>Distribution Files\S1984\MecE_265_Aryanci\MecE_265.xlsx</t>
+  </si>
+  <si>
+    <t>Distribution Files\W2009\MEC E 260 - 502 (77588) Ayranci\MecE260_UNDERGRAD Grade Dist Form.xlsx</t>
   </si>
 </sst>
 </file>
@@ -76,12 +91,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C4"/>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="11.4765625" customWidth="true"/>
     <col min="2" max="2" width="9.7109375" customWidth="true"/>
-    <col min="3" max="3" width="7.890625" customWidth="true"/>
+    <col min="3" max="3" width="82.4765625" customWidth="true"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -89,10 +104,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="2">
@@ -100,10 +115,32 @@
         <v>1</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C2" s="0" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="0" t="s">
         <v>5</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>